<commit_message>
Adding ack to report!
</commit_message>
<xml_diff>
--- a/SmartKitchen-Emdebbed System/Documents/Report/WhatIlearned.xlsx
+++ b/SmartKitchen-Emdebbed System/Documents/Report/WhatIlearned.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Beginner</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t xml:space="preserve">Measurement/test equipment </t>
+  </si>
+  <si>
+    <t>iPi Mocap Studio</t>
+  </si>
+  <si>
+    <t>Hardware/Software debug!</t>
+  </si>
+  <si>
+    <t>Wheatstone bridge weightscale</t>
   </si>
 </sst>
 </file>
@@ -166,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +206,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -434,24 +449,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -465,9 +468,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,482 +780,554 @@
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="8"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="13"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="13"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="13"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="13"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="13"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="13"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="13"/>
+      <c r="A26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="13"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="13"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="13"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="13"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="15"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="B40" s="23"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="11"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1246,7 +1335,7 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A37:I38"/>
+    <mergeCell ref="A43:I44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working Wifitest - connect and read html
</commit_message>
<xml_diff>
--- a/SmartKitchen-Emdebbed System/Documents/Report/WhatIlearned.xlsx
+++ b/SmartKitchen-Emdebbed System/Documents/Report/WhatIlearned.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Beginner</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Wheatstone bridge weightscale</t>
+  </si>
+  <si>
+    <t>M2X AT&amp;T Develop</t>
   </si>
 </sst>
 </file>
@@ -468,6 +471,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,8 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,22 +783,22 @@
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1147,10 +1150,12 @@
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
+      <c r="A29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -1194,24 +1199,24 @@
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="9"/>
@@ -1220,11 +1225,11 @@
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="9"/>
@@ -1233,12 +1238,12 @@
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
       <c r="H36" s="8"/>
       <c r="I36" s="9"/>
     </row>
@@ -1246,12 +1251,12 @@
       <c r="A37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
       <c r="H37" s="8"/>
       <c r="I37" s="9"/>
     </row>
@@ -1259,10 +1264,10 @@
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -1272,12 +1277,12 @@
       <c r="A39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="8"/>
       <c r="I39" s="9"/>
     </row>
@@ -1285,11 +1290,11 @@
       <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="9"/>
@@ -1306,28 +1311,28 @@
       <c r="I41" s="11"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>